<commit_message>
Further updates to the latest two GAs
</commit_message>
<xml_diff>
--- a/Hill Climbing/Hill Climbing experiments.xlsx
+++ b/Hill Climbing/Hill Climbing experiments.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolagheza/Dropbox/DKE/Period 3/PP3/Hill Climbing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Simon\Documents\GitHub\PP3\Hill Climbing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11600" yWindow="460" windowWidth="14000" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="11595" yWindow="465" windowWidth="13995" windowHeight="14715" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -168,13 +168,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -677,23 +680,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
+    <col min="2" max="2" width="13.125" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.375" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" customWidth="1"/>
+    <col min="8" max="8" width="11.625" customWidth="1"/>
+    <col min="10" max="10" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -725,7 +728,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -757,7 +760,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -778,7 +781,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A11" si="0">A3+1</f>
         <v>3</v>
@@ -787,7 +790,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -796,7 +799,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -805,7 +808,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -814,7 +817,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -823,7 +826,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -832,7 +835,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -841,7 +844,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -850,7 +853,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -876,7 +879,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -902,7 +905,7 @@
         <v>3272</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>A16+1</f>
         <v>2</v>
@@ -929,7 +932,7 @@
         <v>15613</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ref="A18:A35" si="1">A17+1</f>
         <v>3</v>
@@ -956,7 +959,7 @@
         <v>12570</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -983,7 +986,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1010,7 +1013,7 @@
         <v>3517</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1037,7 +1040,7 @@
         <v>17244</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1064,7 +1067,7 @@
         <v>64079</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -1091,7 +1094,7 @@
         <v>5551</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1118,7 +1121,7 @@
         <v>40249</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1145,7 +1148,7 @@
         <v>30934</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1172,7 +1175,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1199,7 +1202,7 @@
         <v>131075</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1226,7 +1229,7 @@
         <v>26756</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1253,7 +1256,7 @@
         <v>17299</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1280,7 +1283,7 @@
         <v>19286</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1307,7 +1310,7 @@
         <v>5439</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1334,7 +1337,7 @@
         <v>129570</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1361,7 +1364,7 @@
         <v>4851</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1388,7 +1391,7 @@
         <v>2585</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1415,7 +1418,7 @@
         <v>15876</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>16</v>
       </c>
@@ -1448,7 +1451,7 @@
         <v>27577.35</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
@@ -1477,7 +1480,7 @@
         <v>15613</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -1503,7 +1506,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -1529,7 +1532,7 @@
         <v>68829</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <f>A43+1</f>
         <v>2</v>
@@ -1556,7 +1559,7 @@
         <v>12282</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" ref="A45:A62" si="3">A44+1</f>
         <v>3</v>
@@ -1583,7 +1586,7 @@
         <v>8501</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -1610,7 +1613,7 @@
         <v>518842</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -1637,97 +1640,97 @@
         <v>290504</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>16</v>
       </c>
@@ -1760,7 +1763,7 @@
         <v>179791.6</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>17</v>
       </c>
@@ -1803,14 +1806,14 @@
       <selection activeCell="A27" sqref="A1:H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="8" max="8" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1836,7 +1839,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1862,7 +1865,7 @@
         <v>3272</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>A5+1</f>
         <v>2</v>
@@ -1889,7 +1892,7 @@
         <v>15613</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ref="A7:A24" si="0">A6+1</f>
         <v>3</v>
@@ -1916,7 +1919,7 @@
         <v>12570</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1943,7 +1946,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1970,7 +1973,7 @@
         <v>3517</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1997,7 +2000,7 @@
         <v>17244</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2024,7 +2027,7 @@
         <v>64079</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2051,7 +2054,7 @@
         <v>5551</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2078,7 +2081,7 @@
         <v>40249</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2105,7 +2108,7 @@
         <v>30934</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2132,7 +2135,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2159,7 +2162,7 @@
         <v>131075</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2186,7 +2189,7 @@
         <v>26756</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2213,7 +2216,7 @@
         <v>17299</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2240,7 +2243,7 @@
         <v>19286</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2267,7 +2270,7 @@
         <v>5439</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2294,7 +2297,7 @@
         <v>129570</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2321,7 +2324,7 @@
         <v>4851</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2348,7 +2351,7 @@
         <v>2585</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2375,7 +2378,7 @@
         <v>15876</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
@@ -2408,7 +2411,7 @@
         <v>27577.35</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>